<commit_message>
refactored chrome_option and added new test files
</commit_message>
<xml_diff>
--- a/tests/data/test_files/test_lob.xlsx
+++ b/tests/data/test_files/test_lob.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optum\hm-automation\tests\data\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1903F9-67DC-49DA-8CDE-67905D47F1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBC14D9-51D5-453D-8A8A-97D60E0F925F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Registration" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -513,7 +513,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>